<commit_message>
Updated BOM, dock and toolhead
- Update bom
- Edit dock and toolhead to use microswitch for docksense
</commit_message>
<xml_diff>
--- a/BOM/Lineux Vzbot Bom.xlsx
+++ b/BOM/Lineux Vzbot Bom.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="92">
   <si>
     <t>Vzbot Carriage</t>
   </si>
@@ -251,6 +251,9 @@
   </si>
   <si>
     <t>Umbilical Extrusion Mount</t>
+  </si>
+  <si>
+    <t>m3 washer</t>
   </si>
   <si>
     <t>m5 x 8mm bhcs</t>
@@ -1176,7 +1179,7 @@
         <v>55</v>
       </c>
       <c r="C40" s="11">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="E40" s="9"/>
       <c r="F40" s="11"/>
@@ -1383,9 +1386,9 @@
       </c>
     </row>
     <row r="55">
-      <c r="A55" s="15"/>
+      <c r="A55" s="9"/>
       <c r="B55" s="10" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C55" s="11">
         <v>2.0</v>
@@ -1418,28 +1421,24 @@
     <row r="57">
       <c r="A57" s="15"/>
       <c r="B57" s="10" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="C57" s="11">
         <v>1.0</v>
       </c>
-      <c r="E57" s="9" t="s">
-        <v>78</v>
-      </c>
-      <c r="F57" s="11">
-        <v>1.0</v>
-      </c>
+      <c r="E57" s="9"/>
+      <c r="F57" s="11"/>
     </row>
     <row r="58">
       <c r="A58" s="15"/>
       <c r="B58" s="10" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C58" s="11">
-        <v>3.0</v>
+        <v>1.0</v>
       </c>
       <c r="E58" s="9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F58" s="11">
         <v>1.0</v>
@@ -1448,13 +1447,13 @@
     <row r="59">
       <c r="A59" s="15"/>
       <c r="B59" s="10" t="s">
-        <v>80</v>
+        <v>22</v>
       </c>
       <c r="C59" s="11">
-        <v>10.0</v>
+        <v>2.0</v>
       </c>
       <c r="E59" s="9" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="F59" s="11">
         <v>1.0</v>
@@ -1463,54 +1462,62 @@
     <row r="60">
       <c r="A60" s="15"/>
       <c r="B60" s="10" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C60" s="11">
         <v>1.0</v>
       </c>
-      <c r="E60" s="12" t="s">
-        <v>83</v>
-      </c>
-      <c r="F60" s="13">
-        <v>1.0</v>
-      </c>
+      <c r="E60" s="9"/>
+      <c r="F60" s="11"/>
     </row>
     <row r="61">
       <c r="A61" s="15"/>
       <c r="B61" s="10" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C61" s="11">
-        <v>1.0</v>
-      </c>
-      <c r="E61" s="10"/>
-      <c r="F61" s="10"/>
+        <v>10.0</v>
+      </c>
+      <c r="E61" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="F61" s="11">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="62">
       <c r="A62" s="15"/>
       <c r="B62" s="10" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C62" s="11">
-        <v>2.0</v>
+        <v>1.0</v>
+      </c>
+      <c r="E62" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="F62" s="13">
+        <v>1.0</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="15"/>
       <c r="B63" s="10" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C63" s="11">
-        <v>11.0</v>
-      </c>
+        <v>1.0</v>
+      </c>
+      <c r="E63" s="10"/>
+      <c r="F63" s="10"/>
     </row>
     <row r="64">
       <c r="A64" s="15"/>
       <c r="B64" s="10" t="s">
-        <v>48</v>
+        <v>86</v>
       </c>
       <c r="C64" s="11">
-        <v>4.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="65">
@@ -1519,33 +1526,51 @@
         <v>87</v>
       </c>
       <c r="C65" s="11">
-        <v>1.0</v>
+        <v>11.0</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="15"/>
       <c r="B66" s="10" t="s">
-        <v>88</v>
+        <v>48</v>
       </c>
       <c r="C66" s="11">
-        <v>1.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="15"/>
       <c r="B67" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="C67" s="11">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" s="15"/>
+      <c r="B68" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="C67" s="11">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="68">
-      <c r="A68" s="17"/>
-      <c r="B68" s="14" t="s">
+      <c r="C68" s="11">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" s="15"/>
+      <c r="B69" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="C68" s="13">
+      <c r="C69" s="11">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" s="17"/>
+      <c r="B70" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="C70" s="13">
         <v>1.0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Files Update and Manual released
Updated all CAD
Full Manual released
</commit_message>
<xml_diff>
--- a/BOM/Lineux Vzbot Bom.xlsx
+++ b/BOM/Lineux Vzbot Bom.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="95">
   <si>
     <t>Vzbot Carriage</t>
   </si>
@@ -274,7 +274,7 @@
     <t>Fixed Dock Extrusion Mount L</t>
   </si>
   <si>
-    <t>m4 x 12mm threaded dowel pin ID m3</t>
+    <t>m4 x 15mm threaded dowel pin ID m3</t>
   </si>
   <si>
     <t>m3 t nut</t>
@@ -283,7 +283,10 @@
     <t>m5 t nut</t>
   </si>
   <si>
-    <t>spring OD6 ID5 15mm</t>
+    <t>m5 spring t nut</t>
+  </si>
+  <si>
+    <t>spring OD6 ID5 17mm</t>
   </si>
   <si>
     <t>AA battery terminal</t>
@@ -299,7 +302,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -312,6 +315,10 @@
       <scheme val="minor"/>
     </font>
     <font/>
+    <font>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -397,7 +404,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -441,6 +448,9 @@
     </xf>
     <xf borderId="4" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="5" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="6" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -1390,7 +1400,7 @@
         <v>74</v>
       </c>
       <c r="C55" s="11">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="E55" s="9" t="s">
         <v>75</v>
@@ -1420,7 +1430,7 @@
         <v>77</v>
       </c>
       <c r="C57" s="11">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="E57" s="9" t="s">
         <v>78</v>
@@ -1540,25 +1550,25 @@
         <v>89</v>
       </c>
       <c r="C66" s="11">
-        <v>11.0</v>
+        <v>8.0</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="15"/>
-      <c r="B67" s="10" t="s">
-        <v>50</v>
+      <c r="B67" s="17" t="s">
+        <v>90</v>
       </c>
       <c r="C67" s="11">
-        <v>4.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="15"/>
       <c r="B68" s="10" t="s">
-        <v>90</v>
+        <v>50</v>
       </c>
       <c r="C68" s="11">
-        <v>1.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="69">
@@ -1580,11 +1590,20 @@
       </c>
     </row>
     <row r="71">
-      <c r="A71" s="17"/>
-      <c r="B71" s="14" t="s">
+      <c r="A71" s="15"/>
+      <c r="B71" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="C71" s="13">
+      <c r="C71" s="11">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" s="18"/>
+      <c r="B72" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="C72" s="13">
         <v>1.0</v>
       </c>
     </row>

</xml_diff>